<commit_message>
made changes to excel files
</commit_message>
<xml_diff>
--- a/Resources/amazon_market_capitalization.xlsx
+++ b/Resources/amazon_market_capitalization.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a743a8b7b98e92d/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\03_Data_Engineering_Project\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F783B1E9-B9D8-4974-9402-5468A23B5549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FBC4E4-010E-4B6F-AC74-D864155C65C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4044" yWindow="3900" windowWidth="17280" windowHeight="9072" xr2:uid="{AFB802F6-78E3-4644-86AF-914A4C3411AE}"/>
+    <workbookView xWindow="4560" yWindow="2604" windowWidth="17280" windowHeight="9072" xr2:uid="{AFB802F6-78E3-4644-86AF-914A4C3411AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>$2.008 T</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>$1.44 B</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Market cap</t>
+  </si>
+  <si>
+    <t>Change</t>
   </si>
 </sst>
 </file>
@@ -492,316 +501,327 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{962C3331-A82C-47FD-A913-C262855E77AA}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection sqref="A1:C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>2024</v>
+      <c r="A1" t="s">
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1">
-        <v>0.27929999999999999</v>
+        <v>29</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
-        <v>0.83230000000000004</v>
+        <v>0.27929999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>-0.49320000000000003</v>
+        <v>0.83230000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1">
-        <v>3.4799999999999998E-2</v>
+        <v>-0.49320000000000003</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>0.77580000000000005</v>
+        <v>3.4799999999999998E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1">
-        <v>0.24779999999999999</v>
+        <v>0.77580000000000005</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
-        <v>0.30859999999999999</v>
+        <v>0.24779999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1">
-        <v>0.58160000000000001</v>
+        <v>0.30859999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1">
-        <v>0.1193</v>
+        <v>0.58160000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
-        <v>1.2059</v>
+        <v>0.1193</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1">
-        <v>-0.21160000000000001</v>
+        <v>1.2059</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1">
-        <v>0.60709999999999997</v>
+        <v>-0.21160000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1">
-        <v>0.44690000000000002</v>
+        <v>0.60709999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1">
-        <v>-3.0300000000000001E-2</v>
+        <v>0.44690000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1">
-        <v>0.35920000000000002</v>
+        <v>-3.0300000000000001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1">
-        <v>1.716</v>
+        <v>0.35920000000000002</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1">
-        <v>-0.4294</v>
+        <v>1.716</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1">
-        <v>1.359</v>
+        <v>-0.4294</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1">
-        <v>-0.1671</v>
+        <v>1.359</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1">
-        <v>8.09E-2</v>
+        <v>-0.1671</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1">
-        <v>-0.14499999999999999</v>
+        <v>8.09E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1">
-        <v>1.8965000000000001</v>
+        <v>-0.14499999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1">
-        <v>0.8145</v>
+        <v>1.8965000000000001</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1">
-        <v>-0.27339999999999998</v>
+        <v>0.8145</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="1">
-        <v>-0.78849999999999998</v>
+        <v>-0.27339999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="1">
-        <v>0.54059999999999997</v>
+        <v>-0.78849999999999998</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="1">
-        <v>10.8134</v>
+        <v>0.54059999999999997</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
+        <v>1998</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="1">
+        <v>10.8134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>1997</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finalized market cap csv
</commit_message>
<xml_diff>
--- a/Resources/amazon_market_capitalization.xlsx
+++ b/Resources/amazon_market_capitalization.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\03_Data_Engineering_Project\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nestor\Documents\Bootcamp\Repos\Projects\03_Data_Engineering_Project\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FBC4E4-010E-4B6F-AC74-D864155C65C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC01151-53F9-4EB9-BD70-45156EBE4E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4560" yWindow="2604" windowWidth="17280" windowHeight="9072" xr2:uid="{AFB802F6-78E3-4644-86AF-914A4C3411AE}"/>
+    <workbookView xWindow="29130" yWindow="750" windowWidth="28110" windowHeight="14130" xr2:uid="{AFB802F6-78E3-4644-86AF-914A4C3411AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -125,10 +123,10 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Market cap</t>
-  </si>
-  <si>
     <t>Change</t>
+  </si>
+  <si>
+    <t>MarketCap</t>
   </si>
 </sst>
 </file>
@@ -504,23 +502,26 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C29"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
       <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -531,7 +532,7 @@
         <v>0.27929999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2023</v>
       </c>
@@ -542,7 +543,7 @@
         <v>0.83230000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -553,7 +554,7 @@
         <v>-0.49320000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -564,7 +565,7 @@
         <v>3.4799999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2020</v>
       </c>
@@ -575,7 +576,7 @@
         <v>0.77580000000000005</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2019</v>
       </c>
@@ -586,7 +587,7 @@
         <v>0.24779999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -597,7 +598,7 @@
         <v>0.30859999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -608,7 +609,7 @@
         <v>0.58160000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2016</v>
       </c>
@@ -619,7 +620,7 @@
         <v>0.1193</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2015</v>
       </c>
@@ -630,7 +631,7 @@
         <v>1.2059</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2014</v>
       </c>
@@ -641,7 +642,7 @@
         <v>-0.21160000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2013</v>
       </c>
@@ -652,7 +653,7 @@
         <v>0.60709999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2012</v>
       </c>
@@ -663,7 +664,7 @@
         <v>0.44690000000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -674,7 +675,7 @@
         <v>-3.0300000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2010</v>
       </c>
@@ -685,7 +686,7 @@
         <v>0.35920000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2009</v>
       </c>
@@ -696,7 +697,7 @@
         <v>1.716</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2008</v>
       </c>
@@ -707,7 +708,7 @@
         <v>-0.4294</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2007</v>
       </c>
@@ -718,7 +719,7 @@
         <v>1.359</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2006</v>
       </c>
@@ -729,7 +730,7 @@
         <v>-0.1671</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2005</v>
       </c>
@@ -740,7 +741,7 @@
         <v>8.09E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2004</v>
       </c>
@@ -751,7 +752,7 @@
         <v>-0.14499999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2003</v>
       </c>
@@ -762,7 +763,7 @@
         <v>1.8965000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2002</v>
       </c>
@@ -773,7 +774,7 @@
         <v>0.8145</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2001</v>
       </c>
@@ -784,7 +785,7 @@
         <v>-0.27339999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2000</v>
       </c>
@@ -795,7 +796,7 @@
         <v>-0.78849999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1999</v>
       </c>
@@ -806,7 +807,7 @@
         <v>0.54059999999999997</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1998</v>
       </c>
@@ -817,7 +818,7 @@
         <v>10.8134</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1997</v>
       </c>

</xml_diff>